<commit_message>
Setup Kegiatan: insert perserta dan  uh untuk masing2 peserta di tabel uhDalamNegeri dan uhLuarNegeri
</commit_message>
<xml_diff>
--- a/docs/template-excel/peserta.xlsx
+++ b/docs/template-excel/peserta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fathurrohman/Proyek/honorarium/source-code/honorarium/public/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FATHUR\KERJAAN\pembanding\panda\docs\template-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60193F3A-D56C-194F-981D-76B4EA4594F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA39BA7-F878-4BE5-9C83-8EBE16B9178A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19500" xr2:uid="{674168BC-6BCF-C342-9E35-C2DEB8BAE251}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{674168BC-6BCF-C342-9E35-C2DEB8BAE251}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -186,6 +186,36 @@
   </si>
   <si>
     <t>NPWP</t>
+  </si>
+  <si>
+    <t>Golongan UH LN</t>
+  </si>
+  <si>
+    <t>Pak Menteri Fulan</t>
+  </si>
+  <si>
+    <t>1234567899877777</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Pak Golongan B</t>
+  </si>
+  <si>
+    <t>1234567899877799</t>
+  </si>
+  <si>
+    <t>Duta Besar</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>30302</t>
+  </si>
+  <si>
+    <t>Menteri</t>
   </si>
 </sst>
 </file>
@@ -278,9 +308,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -318,7 +348,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -424,7 +454,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -566,7 +596,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -583,25 +613,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236FD699-9766-F24C-9067-529CD1A244A0}">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -627,19 +660,22 @@
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -662,20 +698,21 @@
         <v>16</v>
       </c>
       <c r="H2" s="2"/>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -700,20 +737,21 @@
       <c r="H3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="2"/>
+      <c r="J3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -736,93 +774,154 @@
         <v>17</v>
       </c>
       <c r="H4" s="2"/>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="2"/>
+      <c r="J4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="O5" t="s">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="P5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="O6" t="s">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="2">
+        <v>31111</v>
+      </c>
+      <c r="P6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="O7" t="s">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="O8" t="s">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="O9" t="s">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="O10" t="s">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="O11" t="s">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="O12" t="s">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="O13" t="s">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="O14" t="s">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="O15" t="s">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="O16" t="s">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P16" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="15:15" x14ac:dyDescent="0.2">
-      <c r="O17" t="s">
+    <row r="17" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P17" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="15:15" x14ac:dyDescent="0.2">
-      <c r="O18" t="s">
+    <row r="18" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P18" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Golongan/Ruang" error="Data tidak benar" sqref="F1:F1048576" xr:uid="{CBF6BBEA-9FEE-8D40-A62B-DF44C4B864C2}">
-      <formula1>$O$2:$O$18</formula1>
+      <formula1>$P$2:$P$18</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Excel Peserta: tambah kolom Berangkat dan Kembali
</commit_message>
<xml_diff>
--- a/docs/template-excel/peserta.xlsx
+++ b/docs/template-excel/peserta.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FATHUR\KERJAAN\pembanding\panda\docs\template-excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fathurrohman/Proyek/honorarium/source-code/panda/docs/template-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA39BA7-F878-4BE5-9C83-8EBE16B9178A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265E15FE-0533-2C41-97F4-EDE593C7F816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{674168BC-6BCF-C342-9E35-C2DEB8BAE251}"/>
+    <workbookView xWindow="-28800" yWindow="4100" windowWidth="28800" windowHeight="17500" xr2:uid="{674168BC-6BCF-C342-9E35-C2DEB8BAE251}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -54,10 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
-  <si>
-    <t>ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
   <si>
     <t>Nama</t>
   </si>
@@ -98,9 +95,6 @@
     <t>III/c</t>
   </si>
   <si>
-    <t>II</t>
-  </si>
-  <si>
     <t>Kepala Pusdiklat</t>
   </si>
   <si>
@@ -216,12 +210,24 @@
   </si>
   <si>
     <t>Menteri</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Berangkat</t>
+  </si>
+  <si>
+    <t>Kembali</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -279,11 +285,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -308,9 +317,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -348,7 +357,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -454,7 +463,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -596,7 +605,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -613,315 +622,352 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236FD699-9766-F24C-9067-529CD1A244A0}">
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomRight" activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="14.33203125" style="6" customWidth="1"/>
+    <col min="12" max="12" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="P2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J2" s="5">
+        <v>45586</v>
+      </c>
+      <c r="K2" s="5">
+        <v>45649</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="H3" s="2">
+        <v>2</v>
       </c>
       <c r="I3" s="2"/>
-      <c r="J3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" s="2" t="s">
+      <c r="J3" s="5">
+        <v>45587</v>
+      </c>
+      <c r="K3" s="5">
+        <v>45650</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="P3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J4" s="5">
+        <v>45588</v>
+      </c>
+      <c r="K4" s="5">
+        <v>45651</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="R4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="P5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J5" s="5">
+        <v>45589</v>
+      </c>
+      <c r="K5" s="5">
+        <v>45652</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="R5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L6" s="2">
+        <v>49</v>
+      </c>
+      <c r="J6" s="5">
+        <v>45590</v>
+      </c>
+      <c r="K6" s="5">
+        <v>45653</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" s="2">
         <v>31111</v>
       </c>
-      <c r="P6" t="s">
+      <c r="R6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="P7" t="s">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="P8" t="s">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="P9" t="s">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="P10" t="s">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="P11" t="s">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="P12" t="s">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="P13" t="s">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="P14" t="s">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R16" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="P15" t="s">
+    <row r="17" spans="18:18" x14ac:dyDescent="0.2">
+      <c r="R17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="P16" t="s">
+    <row r="18" spans="18:18" x14ac:dyDescent="0.2">
+      <c r="R18" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P18" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Golongan/Ruang" error="Data tidak benar" sqref="F1:F1048576" xr:uid="{CBF6BBEA-9FEE-8D40-A62B-DF44C4B864C2}">
-      <formula1>$P$2:$P$18</formula1>
+      <formula1>$R$2:$R$18</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update login error message
</commit_message>
<xml_diff>
--- a/docs/template-excel/peserta.xlsx
+++ b/docs/template-excel/peserta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fathurrohman/Proyek/honorarium/source-code/panda/docs/template-excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FATHUR\KERJAAN\Proyek-Honorarium\dokumen-upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265E15FE-0533-2C41-97F4-EDE593C7F816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459A2104-3033-4A2D-A78E-35F7D7EAAB7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="4100" windowWidth="28800" windowHeight="17500" xr2:uid="{674168BC-6BCF-C342-9E35-C2DEB8BAE251}"/>
+    <workbookView xWindow="31215" yWindow="6240" windowWidth="23070" windowHeight="8130" xr2:uid="{674168BC-6BCF-C342-9E35-C2DEB8BAE251}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,15 +74,6 @@
     <t>Bank</t>
   </si>
   <si>
-    <t>Ayam</t>
-  </si>
-  <si>
-    <t>Bebek</t>
-  </si>
-  <si>
-    <t>Angsa</t>
-  </si>
-  <si>
     <t>111111</t>
   </si>
   <si>
@@ -219,6 +210,15 @@
   </si>
   <si>
     <t>Kembali</t>
+  </si>
+  <si>
+    <t>Abimanyu</t>
+  </si>
+  <si>
+    <t>Kresna</t>
+  </si>
+  <si>
+    <t>Bisma</t>
   </si>
 </sst>
 </file>
@@ -228,7 +228,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -239,6 +239,12 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -317,9 +323,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -357,7 +363,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -463,7 +469,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -605,7 +611,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -628,25 +634,25 @@
       <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O1" sqref="O1"/>
+      <selection pane="bottomRight" activeCell="J1" sqref="J1:K1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="14.33203125" style="6" customWidth="1"/>
-    <col min="12" max="12" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="14.375" style="6" customWidth="1"/>
+    <col min="12" max="12" width="14.125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -655,13 +661,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -670,13 +676,13 @@
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>4</v>
@@ -685,286 +691,287 @@
         <v>5</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="R1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="5">
-        <v>45586</v>
+        <v>45634</v>
       </c>
       <c r="K2" s="5">
-        <v>45649</v>
+        <v>45639</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="R2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="H3" s="2">
         <v>2</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="5">
-        <v>45587</v>
+        <v>45634</v>
       </c>
       <c r="K3" s="5">
-        <v>45650</v>
+        <v>45639</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="R3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="5">
-        <v>45588</v>
+        <v>45634</v>
       </c>
       <c r="K4" s="5">
-        <v>45651</v>
+        <v>45639</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="M4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="R4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J5" s="5">
-        <v>45589</v>
+        <v>45634</v>
       </c>
       <c r="K5" s="5">
-        <v>45652</v>
+        <v>45639</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="R5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J6" s="5">
-        <v>45590</v>
+        <v>45634</v>
       </c>
       <c r="K6" s="5">
-        <v>45653</v>
+        <v>45639</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="N6" s="2">
         <v>31111</v>
       </c>
       <c r="R6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="R7" t="s">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="R8" t="s">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="R9" t="s">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="R10" t="s">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="R11" t="s">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="R12" t="s">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="R13" t="s">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="R14" t="s">
+    <row r="17" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="R15" t="s">
+    <row r="18" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="R16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="18:18" x14ac:dyDescent="0.2">
-      <c r="R17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="18:18" x14ac:dyDescent="0.2">
-      <c r="R18" t="s">
-        <v>38</v>
-      </c>
-    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Golongan/Ruang" error="Data tidak benar" sqref="F1:F1048576" xr:uid="{CBF6BBEA-9FEE-8D40-A62B-DF44C4B864C2}">
       <formula1>$R$2:$R$18</formula1>

</xml_diff>